<commit_message>
Finished the v1 code
</commit_message>
<xml_diff>
--- a/BOM Arduino Doorlock.xlsx
+++ b/BOM Arduino Doorlock.xlsx
@@ -554,7 +554,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -565,7 +565,7 @@
   <dimension ref="B1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,7 +633,7 @@
         <v>10000</v>
       </c>
       <c r="G5" s="20"/>
-      <c r="H5" s="22" t="s">
+      <c r="H5" s="23" t="s">
         <v>16</v>
       </c>
     </row>
@@ -652,7 +652,7 @@
         <v>6000</v>
       </c>
       <c r="G6" s="20"/>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="23" t="s">
         <v>18</v>
       </c>
     </row>
@@ -699,7 +699,7 @@
         <v>21000</v>
       </c>
       <c r="G9" s="20"/>
-      <c r="H9" s="22" t="s">
+      <c r="H9" s="23" t="s">
         <v>20</v>
       </c>
     </row>
@@ -756,7 +756,7 @@
         <v>15000</v>
       </c>
       <c r="G12" s="20"/>
-      <c r="H12" s="22" t="s">
+      <c r="H12" s="23" t="s">
         <v>25</v>
       </c>
     </row>
@@ -866,8 +866,12 @@
     <hyperlink ref="H10" r:id="rId1"/>
     <hyperlink ref="H11" r:id="rId2"/>
     <hyperlink ref="H13" r:id="rId3"/>
+    <hyperlink ref="H5" r:id="rId4"/>
+    <hyperlink ref="H6" r:id="rId5"/>
+    <hyperlink ref="H9" r:id="rId6"/>
+    <hyperlink ref="H12" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>